<commit_message>
EDIT -- Perubahan Format Penggajian parttimer
</commit_message>
<xml_diff>
--- a/public/FORMAT IMPORT DATA PARTTIMER.xlsx
+++ b/public/FORMAT IMPORT DATA PARTTIMER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/projek/hcm2/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F0860D-D410-F349-B6D4-FFC0D77E3441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A06E627-4BF4-C146-B57D-C498FD6420A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16760" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
   <si>
     <t>no</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Iki</t>
   </si>
   <si>
-    <t>GAJI</t>
-  </si>
-  <si>
     <t>Total Remun</t>
   </si>
   <si>
@@ -167,25 +164,31 @@
     <t>PS/ Double Job</t>
   </si>
   <si>
-    <t>Total Point potongan Absensi</t>
-  </si>
-  <si>
     <t>STATUS KEPEGAWAIAN</t>
   </si>
   <si>
     <t>Potongan Koperasi</t>
   </si>
   <si>
-    <t xml:space="preserve"> Jumlah Kehadiran </t>
-  </si>
-  <si>
-    <t>noaa</t>
-  </si>
-  <si>
-    <t>npwps</t>
-  </si>
-  <si>
-    <t>Upah Per Kehadiran / Shift</t>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Transportasi</t>
+  </si>
+  <si>
+    <t>MANGKIR</t>
+  </si>
+  <si>
+    <t>TELAT</t>
+  </si>
+  <si>
+    <t>npwpW</t>
+  </si>
+  <si>
+    <t>noW</t>
+  </si>
+  <si>
+    <t>Gaji Pokok</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
   <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -260,17 +263,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA2"/>
+  <dimension ref="A1:BB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AP9" sqref="AP9"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -578,24 +584,27 @@
     <col min="27" max="27" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.6640625" customWidth="1"/>
     <col min="29" max="29" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.6640625" customWidth="1"/>
-    <col min="49" max="49" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.33203125" customWidth="1"/>
-    <col min="51" max="51" width="26.33203125" customWidth="1"/>
-    <col min="52" max="52" width="3.5" customWidth="1"/>
+    <col min="30" max="30" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.6640625" customWidth="1"/>
+    <col min="50" max="50" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.33203125" customWidth="1"/>
+    <col min="52" max="52" width="26.33203125" customWidth="1"/>
+    <col min="53" max="53" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -663,90 +672,96 @@
         <v>21</v>
       </c>
       <c r="W1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>49</v>
@@ -769,7 +784,7 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J2" t="s">
@@ -811,86 +826,256 @@
       <c r="V2" t="s">
         <v>21</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" t="s">
         <v>22</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="AA2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="BA2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5">
+        <v>5</v>
+      </c>
+      <c r="G3" s="5">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5">
+        <v>7</v>
+      </c>
+      <c r="I3" s="5">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5">
+        <v>9</v>
+      </c>
+      <c r="K3" s="5">
+        <v>10</v>
+      </c>
+      <c r="L3" s="5">
+        <v>11</v>
+      </c>
+      <c r="M3" s="5">
+        <v>12</v>
+      </c>
+      <c r="N3" s="5">
+        <v>13</v>
+      </c>
+      <c r="O3" s="5">
+        <v>14</v>
+      </c>
+      <c r="P3" s="5">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>16</v>
+      </c>
+      <c r="R3" s="5">
+        <v>17</v>
+      </c>
+      <c r="S3" s="5">
+        <v>18</v>
+      </c>
+      <c r="T3" s="5">
+        <v>19</v>
+      </c>
+      <c r="U3" s="5">
+        <v>20</v>
+      </c>
+      <c r="V3" s="5">
+        <v>21</v>
+      </c>
+      <c r="W3" s="5">
+        <v>22</v>
+      </c>
+      <c r="X3" s="5">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="5">
         <v>24</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="Z3" s="5">
         <v>25</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AA3" s="5">
         <v>26</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AB3" s="5">
         <v>27</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AC3" s="5">
         <v>28</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AD3" s="5">
         <v>29</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AE3" s="5">
         <v>30</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AF3" s="5">
         <v>31</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AG3" s="5">
         <v>32</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AH3" s="5">
         <v>33</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AI3" s="5">
         <v>34</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AJ3" s="5">
         <v>35</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AK3" s="5">
         <v>36</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AL3" s="5">
         <v>37</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AM3" s="5">
         <v>38</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AN3" s="5">
         <v>39</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AO3" s="5">
+        <v>40</v>
+      </c>
+      <c r="AP3" s="5">
+        <v>41</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>42</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>43</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>44</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>45</v>
+      </c>
+      <c r="AU3" s="5">
         <v>46</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>44</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>45</v>
+      <c r="AV3" s="5">
+        <v>47</v>
+      </c>
+      <c r="AW3" s="5">
+        <v>48</v>
+      </c>
+      <c r="AX3" s="5">
+        <v>49</v>
+      </c>
+      <c r="AY3" s="5">
+        <v>50</v>
+      </c>
+      <c r="AZ3" s="5">
+        <v>51</v>
+      </c>
+      <c r="BA3" s="5">
+        <v>52</v>
+      </c>
+      <c r="BB3" s="5">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>